<commit_message>
moved extension and delimiter from file_list metadata.xlsx to file_list.xlsx
</commit_message>
<xml_diff>
--- a/excel_files/file_list.xlsx
+++ b/excel_files/file_list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>file1</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t>/Users/krishanuroy/Desktop/Files</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>source_separator</t>
+  </si>
+  <si>
+    <t>target_separator</t>
+  </si>
+  <si>
+    <t>source_extension</t>
+  </si>
+  <si>
+    <t>target_extension</t>
+  </si>
+  <si>
+    <t>csv</t>
   </si>
 </sst>
 </file>
@@ -372,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -384,9 +405,13 @@
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -399,8 +424,20 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -415,8 +452,20 @@
         <f>variables!A2&amp;"/file1_target"</f>
         <v>/Users/krishanuroy/Desktop/Files/file1_target</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -430,6 +479,18 @@
       <c r="D3" t="str">
         <f>variables!A2&amp;"/file2_target"</f>
         <v>/Users/krishanuroy/Desktop/Files/file2_target</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renaming implemented in metadata injection
</commit_message>
<xml_diff>
--- a/excel_files/file_list.xlsx
+++ b/excel_files/file_list.xlsx
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>file1</t>
   </si>
   <si>
-    <t>file2</t>
-  </si>
-  <si>
     <t>file_names</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
   </si>
   <si>
     <t>file1_target</t>
-  </si>
-  <si>
-    <t>file2_target</t>
   </si>
   <si>
     <t>sheet location</t>
@@ -393,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,28 +407,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -442,7 +436,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="str">
         <f>variables!A2&amp;"/file1.csv"</f>
@@ -453,44 +447,16 @@
         <v>/Users/krishanuroy/Desktop/Files/file1_target</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="str">
-        <f>variables!A2&amp;"/file2.txt"</f>
-        <v>/Users/krishanuroy/Desktop/Files/file2.txt</v>
-      </c>
-      <c r="D3" t="str">
-        <f>variables!A2&amp;"/file2_target"</f>
-        <v>/Users/krishanuroy/Desktop/Files/file2_target</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -513,12 +479,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>